<commit_message>
college name also added
</commit_message>
<xml_diff>
--- a/attendance_template.xlsx
+++ b/attendance_template.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,15 +434,20 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>College</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>TotalAttendance</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Feedback</t>
         </is>
@@ -461,13 +466,18 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>ABC College</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>john@example.com</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>15</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Great progress</t>
         </is>
@@ -486,13 +496,18 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>XYZ Institute</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>jane@example.com</t>
         </is>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>14</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Needs improvement</t>
         </is>
@@ -511,13 +526,18 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>ABC College</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>bob@example.com</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>16</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Excellent attendance</t>
         </is>
@@ -536,15 +556,350 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>LMN University</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>alice@example.com</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>13</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Average</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Charlie Ray</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>105</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>XYZ Institute</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>charlie@example.com</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>12</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Can do better</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Diana Prince</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>106</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ABC College</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>diana@example.com</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>17</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Outstanding</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Ethan Hunt</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>107</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>LMN University</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>ethan@example.com</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>11</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Irregular</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Fiona Glen</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>108</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>XYZ Institute</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>fiona@example.com</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>14</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Consistent</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>George White</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>109</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ABC College</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>george@example.com</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>13</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Good effort</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Hannah Moore</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>LMN University</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>hannah@example.com</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>15</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Well done</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Ian Scott</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>111</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>XYZ Institute</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>ian@example.com</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>16</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Punctual</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Julia Chen</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>112</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ABC College</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>julia@example.com</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>12</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Could improve</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Kevin Brooks</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>113</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>LMN University</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>kevin@example.com</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Needs attention</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Laura King</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>114</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>XYZ Institute</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>laura@example.com</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>14</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Steady progress</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Michael Roy</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ABC College</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>michael@example.com</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>15</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Very active</t>
         </is>
       </c>
     </row>

</xml_diff>